<commit_message>
Merged PR 514: Fixed the bug which prevents drawing of acetylide. Also now fixed a bug in th...
Fixed the bug which prevents drawing of acetylide. Also now fixed a bug in the original C4W code when searching for valences

Related work items: #960
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://konecranes1-my.sharepoint.com/personal/mike_williams_tba_group/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-2\src\Chemistry\Chem4Word.Model2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{1FFC7CC2-E339-43C6-8D00-D448709F321E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FF2F3E8-D701-4C01-8F8E-92B4CEAEDBEF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6830BE6E-8428-420C-BC37-E14EFF5A2CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8415" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="524">
   <si>
     <t>Symbol</t>
   </si>
@@ -1600,6 +1604,9 @@
   </si>
   <si>
     <t>Rn 5f14 6d3 7s2</t>
+  </si>
+  <si>
+    <t>3|5|7</t>
   </si>
 </sst>
 </file>
@@ -2454,7 +2461,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3607,7 +3614,7 @@
         <v>30.973762000000001</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>43</v>
+        <v>523</v>
       </c>
       <c r="L22">
         <v>15</v>

</xml_diff>